<commit_message>
Tests adjusted to new functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTests/customersTest.xlsx
+++ b/src/test/resources/excelTests/customersTest.xlsx
@@ -15,14 +15,14 @@
     <sheet name="CUSTOMERS" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CUSTOMERS!$A$2:$I$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CUSTOMERS!$A$2:$J$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -169,6 +169,21 @@
   </si>
   <si>
     <t>KLNMOPwer</t>
+  </si>
+  <si>
+    <t>Time Zone</t>
+  </si>
+  <si>
+    <t>GMT+05</t>
+  </si>
+  <si>
+    <t>GMT+06</t>
+  </si>
+  <si>
+    <t>GMT+07</t>
+  </si>
+  <si>
+    <t>GMT+02</t>
   </si>
 </sst>
 </file>
@@ -213,7 +228,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -326,11 +341,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -353,6 +383,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -633,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,9 +678,10 @@
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -674,11 +706,14 @@
       <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -687,9 +722,10 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
-      <c r="I2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="7"/>
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -714,11 +750,14 @@
       <c r="H3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="2" t="b">
+      <c r="I3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -743,11 +782,14 @@
       <c r="H4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="2" t="b">
+      <c r="I4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -772,11 +814,14 @@
       <c r="H5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="2" t="b">
+      <c r="I5" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -801,11 +846,14 @@
       <c r="H6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="2" t="b">
+      <c r="I6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -830,11 +878,14 @@
       <c r="H7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="2" t="b">
+      <c r="I7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -857,11 +908,14 @@
       <c r="H8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="2" t="b">
+      <c r="I8" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
         <v>38</v>
@@ -878,11 +932,14 @@
         <v>37</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -897,11 +954,14 @@
       <c r="H10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="2" t="b">
+      <c r="I10" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>48</v>
@@ -924,11 +984,14 @@
       <c r="H11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="2" t="b">
+      <c r="I11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2">
@@ -945,22 +1008,24 @@
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2" t="b">
+      <c r="I12" s="2"/>
+      <c r="J12" s="2" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I2"/>
-  <mergeCells count="9">
+  <autoFilter ref="A2:J2"/>
+  <mergeCells count="10">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>